<commit_message>
Added and finished Diplom
</commit_message>
<xml_diff>
--- a/Diplom/diplom.xlsx
+++ b/Diplom/diplom.xlsx
@@ -2,21 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8070" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="First list" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -46,11 +48,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,241 +417,117 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="10.5703125" customWidth="1" min="1" max="1"/>
+    <col width="16.7109375" customWidth="1" min="2" max="2"/>
+    <col width="15.28515625" customWidth="1" min="3" max="3"/>
+    <col width="19.140625" customWidth="1" min="4" max="4"/>
+    <col width="16.42578125" customWidth="1" min="5" max="5"/>
+    <col width="12.85546875" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>Ім'я</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Прізвище</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>По батькові</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>День народження</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>День смерті</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>m</t>
+          <t>Стать</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Вік</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>Андрій</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>Маслов</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>i</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>Вікторович</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>37002</v>
+      </c>
+      <c r="E2" s="1" t="n"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
+          <t>чоловік</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>l</t>
-        </is>
-      </c>
+      <c r="D3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>Юлія</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>Павленко</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>t</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>Семенівна</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>36019</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>e</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>i</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>v</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>i</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>i</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
+          <t>жінка</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>